<commit_message>
feat : npc SO
</commit_message>
<xml_diff>
--- a/tuningdat/ResourceDataSheet.xlsx
+++ b/tuningdat/ResourceDataSheet.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\gitThings\Wonder\2024-Spring-Capstone-team20\tuningdat\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSY\Desktop\2024-Spring-Capstone-team20\tuningdat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2849C0-579C-450C-BBDC-257CF025265A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA3A9E3-28B7-4E75-ABFF-F307D59BF8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{FA097364-AAAC-432F-BD4B-669E1A2F3865}"/>
+    <workbookView xWindow="14265" yWindow="2070" windowWidth="11775" windowHeight="11385" xr2:uid="{FA097364-AAAC-432F-BD4B-669E1A2F3865}"/>
   </bookViews>
   <sheets>
     <sheet name="캐릭터" sheetId="1" r:id="rId1"/>
@@ -21,23 +21,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="52">
   <si>
     <t>relationProb</t>
   </si>
@@ -182,6 +171,34 @@
   </si>
   <si>
     <t>NpcProblemInfo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NpcName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tom</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Jerry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Merry</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Guy</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Boy</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -565,157 +582,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9366EE7-3920-4193-BA89-954AB8B0FB81}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
       <c r="B1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" t="s">
         <v>40</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>41</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>43</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1">
+      <c r="D2" s="1">
         <v>19</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1">
+      <c r="D3" s="1">
         <v>32</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>24</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="1">
+      <c r="D5" s="1">
         <v>19</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="1">
+      <c r="D6" s="1">
         <v>32</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="1">
+      <c r="D7" s="1">
         <v>27</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>38</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>1</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>36</v>
       </c>
     </row>
@@ -733,14 +771,14 @@
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="67.19921875" customWidth="1"/>
-    <col min="4" max="4" width="10.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.25" customWidth="1"/>
+    <col min="4" max="4" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -760,7 +798,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -780,7 +818,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -800,7 +838,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -820,7 +858,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -840,7 +878,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -860,7 +898,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -880,7 +918,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -900,7 +938,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>

</xml_diff>